<commit_message>
1)US28 29.    2)modified unittests to  adapt to new command structure in command line
</commit_message>
<xml_diff>
--- a/Team_1_Report.xlsx
+++ b/Team_1_Report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView windowWidth="22095" windowHeight="12270" tabRatio="768" activeTab="6"/>
+    <workbookView windowWidth="20820" windowHeight="12270" tabRatio="768" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -648,11 +648,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="0.0"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="m/d"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="0.0"/>
+    <numFmt numFmtId="177" formatCode="m/d"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -692,14 +692,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -728,14 +736,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -743,7 +758,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -758,7 +773,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -780,20 +803,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -812,23 +821,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -855,7 +855,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -867,169 +1029,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1040,6 +1040,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1054,59 +1069,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1127,164 +1092,199 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1315,22 +1315,22 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="179" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="10" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -4400,12 +4400,12 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
-    <col min="2" max="2" width="22.6666666666667" customWidth="1"/>
+    <col min="2" max="2" width="28.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1" spans="1:9">
@@ -4566,6 +4566,12 @@
       <c r="F6">
         <v>30</v>
       </c>
+      <c r="G6">
+        <v>21</v>
+      </c>
+      <c r="H6">
+        <v>30</v>
+      </c>
       <c r="I6" s="12">
         <v>42313</v>
       </c>
@@ -4587,6 +4593,12 @@
         <v>20</v>
       </c>
       <c r="F7">
+        <v>30</v>
+      </c>
+      <c r="G7">
+        <v>25</v>
+      </c>
+      <c r="H7">
         <v>30</v>
       </c>
       <c r="I7" s="12">
@@ -5065,8 +5077,8 @@
   <sheetPr/>
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" outlineLevelCol="2"/>

</xml_diff>

<commit_message>
unittest for US33 and US34
</commit_message>
<xml_diff>
--- a/Team_1_Report.xlsx
+++ b/Team_1_Report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr date1904="1"/>
   <bookViews>
-    <workbookView windowWidth="14400" windowHeight="12270" tabRatio="768" firstSheet="2" activeTab="7"/>
+    <workbookView windowWidth="18990" windowHeight="12270" tabRatio="768" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="207">
   <si>
     <t>Initials</t>
   </si>
@@ -650,12 +650,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="0.0"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="m/d"/>
-    <numFmt numFmtId="179" formatCode="0.0"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="m/d"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -702,6 +702,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -709,9 +717,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -725,14 +754,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
@@ -741,7 +762,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -756,7 +784,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -764,16 +792,17 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -794,44 +823,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -858,13 +858,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -876,7 +876,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -888,37 +912,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -936,13 +954,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -954,7 +966,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -966,13 +996,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -984,55 +1026,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1043,6 +1043,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1064,28 +1088,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1105,193 +1124,174 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1315,25 +1315,28 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="179" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="179" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="10" applyAlignment="1"/>
   </cellXfs>
@@ -2554,7 +2557,7 @@
       <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="25" t="s">
         <v>8</v>
       </c>
       <c r="E3" t="s">
@@ -2571,7 +2574,7 @@
       <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="25" t="s">
         <v>13</v>
       </c>
       <c r="E4" t="s">
@@ -2588,7 +2591,7 @@
       <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="26" t="s">
         <v>18</v>
       </c>
       <c r="E5" t="s">
@@ -2605,7 +2608,7 @@
       <c r="C6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="26" t="s">
         <v>23</v>
       </c>
       <c r="E6" t="s">
@@ -2622,7 +2625,7 @@
       <c r="C7" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="26" t="s">
         <v>28</v>
       </c>
       <c r="E7" t="s">
@@ -2659,7 +2662,7 @@
   <sheetPr/>
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" topLeftCell="A21" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" topLeftCell="A31" workbookViewId="0">
       <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
@@ -3421,41 +3424,41 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="10.8333333333333" style="14"/>
+    <col min="1" max="1" width="10.8333333333333" style="15"/>
     <col min="2" max="2" width="9.5" customWidth="1"/>
     <col min="3" max="3" width="15.8333333333333" customWidth="1"/>
     <col min="4" max="4" width="12.3333333333333" customWidth="1"/>
     <col min="5" max="5" width="6.83333333333333" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="17" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="15" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="15" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="15" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="15" t="s">
         <v>127</v>
       </c>
     </row>
@@ -3463,7 +3466,7 @@
       <c r="A14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="19" t="s">
         <v>128</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -3478,7 +3481,7 @@
       <c r="F14" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="G14" s="19" t="s">
+      <c r="G14" s="20" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3486,114 +3489,114 @@
       <c r="A15" t="s">
         <v>134</v>
       </c>
-      <c r="B15" s="21">
+      <c r="B15" s="22">
         <v>41065</v>
       </c>
-      <c r="C15" s="22">
+      <c r="C15" s="23">
         <v>24</v>
       </c>
-      <c r="E15" s="22">
+      <c r="E15" s="23">
         <v>0</v>
       </c>
-      <c r="F15" s="22"/>
-      <c r="G15" s="17"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="18"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>135</v>
       </c>
-      <c r="B16" s="21">
+      <c r="B16" s="22">
         <v>41078</v>
       </c>
-      <c r="C16" s="22">
+      <c r="C16" s="23">
         <v>18</v>
       </c>
       <c r="D16">
         <f>C15-C16</f>
         <v>6</v>
       </c>
-      <c r="E16" s="22">
+      <c r="E16" s="23">
         <v>250</v>
       </c>
-      <c r="F16" s="22">
+      <c r="F16" s="23">
         <v>120</v>
       </c>
-      <c r="G16" s="17">
+      <c r="G16" s="18">
         <f>(E16-E15)/F16*60</f>
         <v>125</v>
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="B17" s="21">
+      <c r="B17" s="22">
         <v>41092</v>
       </c>
-      <c r="C17" s="22">
+      <c r="C17" s="23">
         <v>12</v>
       </c>
       <c r="D17">
         <f t="shared" ref="D17:D19" si="0">C16-C17</f>
         <v>6</v>
       </c>
-      <c r="E17" s="22">
+      <c r="E17" s="23">
         <v>480</v>
       </c>
-      <c r="F17" s="23">
+      <c r="F17" s="24">
         <v>135</v>
       </c>
-      <c r="G17" s="17">
+      <c r="G17" s="18">
         <f t="shared" ref="G17:G19" si="1">(E17-E16)/F17*60</f>
         <v>102.222222222222</v>
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="B18" s="21">
+      <c r="B18" s="22">
         <v>41106</v>
       </c>
-      <c r="C18" s="22">
+      <c r="C18" s="23">
         <v>6</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E18" s="22">
+      <c r="E18" s="23">
         <v>740</v>
       </c>
-      <c r="F18" s="23">
+      <c r="F18" s="24">
         <v>160</v>
       </c>
-      <c r="G18" s="17">
+      <c r="G18" s="18">
         <f t="shared" si="1"/>
         <v>97.5</v>
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="B19" s="21">
+      <c r="B19" s="22">
         <v>41120</v>
       </c>
-      <c r="C19" s="22">
+      <c r="C19" s="23">
         <v>0</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E19" s="22">
+      <c r="E19" s="23">
         <v>1100</v>
       </c>
-      <c r="F19" s="23">
+      <c r="F19" s="24">
         <v>145</v>
       </c>
-      <c r="G19" s="17">
+      <c r="G19" s="18">
         <f t="shared" si="1"/>
         <v>148.965517241379</v>
       </c>
@@ -3617,19 +3620,19 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" outlineLevelRow="6" outlineLevelCol="6"/>
   <cols>
-    <col min="2" max="2" width="10.8333333333333" style="14"/>
+    <col min="2" max="2" width="10.8333333333333" style="15"/>
     <col min="3" max="3" width="20.5" customWidth="1"/>
     <col min="4" max="4" width="14.4166666666667" customWidth="1"/>
     <col min="5" max="5" width="7.16666666666667" customWidth="1"/>
     <col min="6" max="6" width="6.83333333333333" customWidth="1"/>
-    <col min="7" max="7" width="13.75" style="17" customWidth="1"/>
+    <col min="7" max="7" width="13.75" style="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="19" t="s">
         <v>128</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -3644,7 +3647,7 @@
       <c r="F1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="20" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3652,7 +3655,7 @@
       <c r="A2" t="s">
         <v>134</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="17">
         <v>42270</v>
       </c>
       <c r="C2" s="10">
@@ -3663,13 +3666,13 @@
         <v>0</v>
       </c>
       <c r="F2" s="10"/>
-      <c r="G2" s="13"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>135</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="17">
         <v>42256</v>
       </c>
       <c r="C3" s="10">
@@ -3684,15 +3687,15 @@
       <c r="F3" s="10">
         <v>270</v>
       </c>
-      <c r="G3" s="20">
+      <c r="G3" s="21">
         <v>41.6</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="17" t="s">
         <v>139</v>
       </c>
       <c r="C4" s="10">
@@ -3707,15 +3710,15 @@
       <c r="F4" s="10">
         <v>300</v>
       </c>
-      <c r="G4" s="20">
+      <c r="G4" s="21">
         <v>46.4</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="17">
         <v>42165</v>
       </c>
       <c r="C5" s="10">
@@ -3730,15 +3733,15 @@
       <c r="F5" s="10">
         <v>245</v>
       </c>
-      <c r="G5" s="20">
+      <c r="G5" s="21">
         <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="17" t="s">
         <v>140</v>
       </c>
       <c r="C6" s="10">
@@ -3749,15 +3752,15 @@
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
-      <c r="G6" s="20"/>
+      <c r="G6" s="21"/>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="16"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
-      <c r="G7" s="20"/>
+      <c r="G7" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3785,7 +3788,7 @@
     <col min="6" max="6" width="9.41666666666667" customWidth="1"/>
     <col min="7" max="7" width="9.08333333333333" customWidth="1"/>
     <col min="8" max="8" width="9.83333333333333" customWidth="1"/>
-    <col min="9" max="9" width="10.8333333333333" style="14"/>
+    <col min="9" max="9" width="10.8333333333333" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -3813,7 +3816,7 @@
       <c r="H1" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="16" t="s">
         <v>145</v>
       </c>
     </row>
@@ -3842,7 +3845,7 @@
       <c r="H2">
         <v>20</v>
       </c>
-      <c r="I2" s="16">
+      <c r="I2" s="17">
         <v>42285</v>
       </c>
     </row>
@@ -3871,7 +3874,7 @@
       <c r="H3">
         <v>10</v>
       </c>
-      <c r="I3" s="16">
+      <c r="I3" s="17">
         <v>42285</v>
       </c>
     </row>
@@ -3900,7 +3903,7 @@
       <c r="H4">
         <v>20</v>
       </c>
-      <c r="I4" s="16">
+      <c r="I4" s="17">
         <v>42285</v>
       </c>
     </row>
@@ -3929,7 +3932,7 @@
       <c r="H5">
         <v>30</v>
       </c>
-      <c r="I5" s="16">
+      <c r="I5" s="17">
         <v>42285</v>
       </c>
     </row>
@@ -3958,7 +3961,7 @@
       <c r="H6">
         <v>30</v>
       </c>
-      <c r="I6" s="16">
+      <c r="I6" s="17">
         <v>42285</v>
       </c>
     </row>
@@ -3987,7 +3990,7 @@
       <c r="H7">
         <v>30</v>
       </c>
-      <c r="I7" s="16">
+      <c r="I7" s="17">
         <v>42285</v>
       </c>
     </row>
@@ -4016,7 +4019,7 @@
       <c r="H8">
         <v>20</v>
       </c>
-      <c r="I8" s="16">
+      <c r="I8" s="17">
         <v>42285</v>
       </c>
     </row>
@@ -4045,7 +4048,7 @@
       <c r="H9">
         <v>20</v>
       </c>
-      <c r="I9" s="16">
+      <c r="I9" s="17">
         <v>42285</v>
       </c>
     </row>
@@ -4074,7 +4077,7 @@
       <c r="H10">
         <v>40</v>
       </c>
-      <c r="I10" s="16">
+      <c r="I10" s="17">
         <v>42285</v>
       </c>
     </row>
@@ -4103,7 +4106,7 @@
       <c r="H11">
         <v>50</v>
       </c>
-      <c r="I11" s="16">
+      <c r="I11" s="17">
         <v>42285</v>
       </c>
     </row>
@@ -4220,7 +4223,7 @@
       <c r="H2">
         <v>30</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="14" t="s">
         <v>152</v>
       </c>
     </row>
@@ -4249,7 +4252,7 @@
       <c r="H3">
         <v>30</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="14" t="s">
         <v>152</v>
       </c>
     </row>
@@ -4278,7 +4281,7 @@
       <c r="H4">
         <v>30</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="14" t="s">
         <v>152</v>
       </c>
     </row>
@@ -4307,7 +4310,7 @@
       <c r="H5">
         <v>30</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="I5" s="14" t="s">
         <v>152</v>
       </c>
     </row>
@@ -4336,7 +4339,7 @@
       <c r="H6">
         <v>30</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="14" t="s">
         <v>152</v>
       </c>
     </row>
@@ -4365,7 +4368,7 @@
       <c r="H7">
         <v>50</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="I7" s="14" t="s">
         <v>152</v>
       </c>
     </row>
@@ -4394,7 +4397,7 @@
       <c r="H8">
         <v>10</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="14" t="s">
         <v>153</v>
       </c>
     </row>
@@ -4423,7 +4426,7 @@
       <c r="H9">
         <v>20</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="14" t="s">
         <v>153</v>
       </c>
     </row>
@@ -4452,7 +4455,7 @@
       <c r="H10">
         <v>40</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="I10" s="14" t="s">
         <v>152</v>
       </c>
     </row>
@@ -4481,7 +4484,7 @@
       <c r="H11">
         <v>30</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="I11" s="14" t="s">
         <v>152</v>
       </c>
     </row>
@@ -4905,13 +4908,20 @@
   <sheetPr/>
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
+    <col min="1" max="1" width="9" customWidth="1"/>
     <col min="2" max="2" width="26.6666666666667" customWidth="1"/>
+    <col min="3" max="3" width="7.41666666666667" customWidth="1"/>
+    <col min="4" max="4" width="8" customWidth="1"/>
+    <col min="5" max="5" width="7.83333333333333" customWidth="1"/>
+    <col min="6" max="6" width="8.83333333333333" customWidth="1"/>
+    <col min="7" max="7" width="9" customWidth="1"/>
+    <col min="8" max="8" width="10.0833333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="16" customHeight="1" spans="1:9">
@@ -5020,9 +5030,7 @@
       <c r="F4">
         <v>30</v>
       </c>
-      <c r="I4" s="10" t="s">
-        <v>158</v>
-      </c>
+      <c r="I4" s="10"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
@@ -5043,9 +5051,7 @@
       <c r="F5">
         <v>30</v>
       </c>
-      <c r="I5" s="10" t="s">
-        <v>158</v>
-      </c>
+      <c r="I5" s="10"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
@@ -5058,7 +5064,7 @@
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>158</v>
+        <v>39</v>
       </c>
       <c r="E6">
         <v>20</v>
@@ -5066,8 +5072,14 @@
       <c r="F6">
         <v>30</v>
       </c>
-      <c r="I6" s="10" t="s">
-        <v>158</v>
+      <c r="G6">
+        <v>20</v>
+      </c>
+      <c r="H6">
+        <v>20</v>
+      </c>
+      <c r="I6" s="13">
+        <v>42326</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -5081,7 +5093,7 @@
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>158</v>
+        <v>39</v>
       </c>
       <c r="E7">
         <v>20</v>
@@ -5089,8 +5101,14 @@
       <c r="F7">
         <v>30</v>
       </c>
-      <c r="I7" s="10" t="s">
-        <v>158</v>
+      <c r="G7">
+        <v>20</v>
+      </c>
+      <c r="H7">
+        <v>20</v>
+      </c>
+      <c r="I7" s="13">
+        <v>42326</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -5112,9 +5130,7 @@
       <c r="F8">
         <v>30</v>
       </c>
-      <c r="I8" s="10" t="s">
-        <v>158</v>
-      </c>
+      <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
@@ -5135,9 +5151,7 @@
       <c r="F9">
         <v>30</v>
       </c>
-      <c r="I9" s="10" t="s">
-        <v>158</v>
-      </c>
+      <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
@@ -5158,9 +5172,7 @@
       <c r="F10">
         <v>30</v>
       </c>
-      <c r="I10" s="10" t="s">
-        <v>158</v>
-      </c>
+      <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
@@ -5181,9 +5193,7 @@
       <c r="F11">
         <v>30</v>
       </c>
-      <c r="I11" s="10" t="s">
-        <v>158</v>
-      </c>
+      <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
@@ -5290,7 +5300,7 @@
   <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" outlineLevelCol="2"/>

</xml_diff>